<commit_message>
(hel-916) Ajout des informations dans le template d’export SAN
</commit_message>
<xml_diff>
--- a/public/templates/template_comparaison_SAN.xlsx
+++ b/public/templates/template_comparaison_SAN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29322"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\webadm\projets\helios\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://catamaniacrm-my.sharepoint.com/personal/y_elhouakmi_catamania_com/Documents/Documents/DNum/Helios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78467E00-9E0B-4CF2-B9EB-D89DF4DDBF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{78467E00-9E0B-4CF2-B9EB-D89DF4DDBF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECA6A6EB-4F37-4DE5-9620-D8B803D62DA7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Indicateurs</t>
   </si>
@@ -525,12 +525,380 @@
 Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.</t>
     </r>
   </si>
+  <si>
+    <t>Nb ETP PM</t>
+  </si>
+  <si>
+    <t>date_mis_a_jour_ancre</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mode de calcul :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Nombre d’équivalents temps pleins moyens rémunérés personnel médical
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Source(s) :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Application Nationale Compte financier Rapport infra-annuel Eprd (ANCRE) - Agence technique de l’information sur l’hospitalisation (ATIH)
+Fichier de la campagne CF.
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
+  <si>
+    <t>Nb ETP PNM</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nombre d’équivalents temps pleins moyens rémunérés personnel non médical
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Application Nationale Compte financier Rapport infra-annuel Eprd (ANCRE) - Agence technique de l’information sur l’hospitalisation (ATIH)
+Fichier de la campagne CF.
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
+  <si>
+    <t>Dépenses intérim PM</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Montant du compte de charge "62113 Personnel intérimaire médical"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Application Nationale Compte financier Rapport infra-annuel Eprd (ANCRE) - Agence technique de l’information sur l’hospitalisation (ATIH)
+Fichier de la campagne CF.
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
+  <si>
+    <t>Jours d’absentéisme PM</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nombre de jours d’absence du personnel médical
+La réalisation du bilan social est obligatoire pour les établissements (qu’ils soient sanitaires, sociaux ou médico-sociaux) dont l’effectif global au 31/12/n-1 est d’au moins 300 agents. Il est facultatif pour les autres établissements.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Enquête « Bilan Social »- Agence technique de l’information sur l’hospitalisation (ATIH)
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
+  <si>
+    <t>Jours d’absentéisme PNM</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nombre de jours d’absence du personnel non médical
+La réalisation du bilan social est obligatoire pour les établissements (qu’ils soient sanitaires, sociaux ou médico-sociaux) dont l’effectif global au 31/12/n-1 est d’au moins 300 agents. Il est facultatif pour les autres établissements.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Enquête « Bilan Social »- Agence technique de l’information sur l’hospitalisation (ATIH)
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -549,6 +917,14 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -572,7 +948,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -591,6 +967,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -931,18 +1310,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587C9ED0-279B-44AC-9485-AC6832055B1B}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="187.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -953,7 +1332,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="48" customHeight="1">
+    <row r="2" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -964,21 +1343,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="31.15">
+    <row r="3" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" ht="309" customHeight="1">
+    <row r="4" spans="1:3" ht="309" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" ht="409.5" customHeight="1">
+    <row r="5" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -989,14 +1368,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="136.5" customHeight="1">
+    <row r="6" spans="1:3" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" ht="274.89999999999998" customHeight="1">
+    <row r="7" spans="1:3" ht="274.89999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1007,7 +1386,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="324">
+    <row r="8" spans="1:3" ht="315" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1018,14 +1397,69 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="240" customHeight="1">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="240" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1047,7 +1481,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
(hel-916) Ajout des nouveaux indicateurs RH à la comparaison d’un ETSAN (#926)
* (hel-916) Ajout des nouveaux indicateurs RH à la comparaison d’un ETSAN

* (hel-916) Fix test

* (hel-916) Ajout des informations dans le template d’export SAN

* (hel-916) Retour PR
</commit_message>
<xml_diff>
--- a/public/templates/template_comparaison_SAN.xlsx
+++ b/public/templates/template_comparaison_SAN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29322"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\webadm\projets\helios\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://catamaniacrm-my.sharepoint.com/personal/y_elhouakmi_catamania_com/Documents/Documents/DNum/Helios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78467E00-9E0B-4CF2-B9EB-D89DF4DDBF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{78467E00-9E0B-4CF2-B9EB-D89DF4DDBF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECA6A6EB-4F37-4DE5-9620-D8B803D62DA7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Indicateurs</t>
   </si>
@@ -525,12 +525,380 @@
 Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.</t>
     </r>
   </si>
+  <si>
+    <t>Nb ETP PM</t>
+  </si>
+  <si>
+    <t>date_mis_a_jour_ancre</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mode de calcul :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Nombre d’équivalents temps pleins moyens rémunérés personnel médical
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Source(s) :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Application Nationale Compte financier Rapport infra-annuel Eprd (ANCRE) - Agence technique de l’information sur l’hospitalisation (ATIH)
+Fichier de la campagne CF.
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
+  <si>
+    <t>Nb ETP PNM</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nombre d’équivalents temps pleins moyens rémunérés personnel non médical
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Application Nationale Compte financier Rapport infra-annuel Eprd (ANCRE) - Agence technique de l’information sur l’hospitalisation (ATIH)
+Fichier de la campagne CF.
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
+  <si>
+    <t>Dépenses intérim PM</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Montant du compte de charge "62113 Personnel intérimaire médical"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Application Nationale Compte financier Rapport infra-annuel Eprd (ANCRE) - Agence technique de l’information sur l’hospitalisation (ATIH)
+Fichier de la campagne CF.
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
+  <si>
+    <t>Jours d’absentéisme PM</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nombre de jours d’absence du personnel médical
+La réalisation du bilan social est obligatoire pour les établissements (qu’ils soient sanitaires, sociaux ou médico-sociaux) dont l’effectif global au 31/12/n-1 est d’au moins 300 agents. Il est facultatif pour les autres établissements.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Enquête « Bilan Social »- Agence technique de l’information sur l’hospitalisation (ATIH)
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
+  <si>
+    <t>Jours d’absentéisme PNM</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fréquence :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Quotidienne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mode de calcul : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nombre de jours d’absence du personnel non médical
+La réalisation du bilan social est obligatoire pour les établissements (qu’ils soient sanitaires, sociaux ou médico-sociaux) dont l’effectif global au 31/12/n-1 est d’au moins 300 agents. Il est facultatif pour les autres établissements.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source(s) :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Enquête « Bilan Social »- Agence technique de l’information sur l’hospitalisation (ATIH)
+Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT qui est un système décisionnel national permettant de stocker des informations provenant de plusieurs sources. DIAMANT : Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -549,6 +917,14 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -572,7 +948,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -591,6 +967,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -931,18 +1310,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587C9ED0-279B-44AC-9485-AC6832055B1B}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="187.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -953,7 +1332,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="48" customHeight="1">
+    <row r="2" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -964,21 +1343,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="31.15">
+    <row r="3" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" ht="309" customHeight="1">
+    <row r="4" spans="1:3" ht="309" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" ht="409.5" customHeight="1">
+    <row r="5" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -989,14 +1368,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="136.5" customHeight="1">
+    <row r="6" spans="1:3" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" ht="274.89999999999998" customHeight="1">
+    <row r="7" spans="1:3" ht="274.89999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1007,7 +1386,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="324">
+    <row r="8" spans="1:3" ht="315" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1018,14 +1397,69 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="240" customHeight="1">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="240" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1047,7 +1481,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>